<commit_message>
chore: add ipynb files
</commit_message>
<xml_diff>
--- a/Thadii banks data set.xlsx
+++ b/Thadii banks data set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Educational\Project\course-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6048FE3-4BEC-4A07-8BEF-094DD9A6F100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF46B022-AE86-41C0-A3B9-B8AC805AD9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6C15A126-5262-EB46-A528-1184AA6210ED}"/>
   </bookViews>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D54ABD-D2A4-4CF6-8E27-1AEC20C43F1B}">
   <dimension ref="A1:K500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>

</xml_diff>